<commit_message>
trials 1D-2D coupling, small change to channel WH cleaned up plot graph for P and Qs linked flod check then no erosion
</commit_message>
<xml_diff>
--- a/docs/floodchannel.xlsx
+++ b/docs/floodchannel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="18">
   <si>
     <t>dx</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>levee</t>
+  </si>
+  <si>
+    <t>if &lt; 0</t>
+  </si>
+  <si>
+    <t>hmx/fc</t>
   </si>
 </sst>
 </file>
@@ -536,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -604,7 +610,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="7">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>4</v>
@@ -614,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="7">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>4</v>
@@ -637,7 +643,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>4</v>
@@ -647,8 +653,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="7">
-        <f>C8</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>4</v>
@@ -659,7 +664,7 @@
       </c>
       <c r="K8" s="7">
         <f>G8</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>4</v>
@@ -673,7 +678,7 @@
       </c>
       <c r="C9" s="9">
         <f>C6-C7</f>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>4</v>
@@ -684,7 +689,7 @@
       </c>
       <c r="G9" s="9">
         <f>G6-G7</f>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>4</v>
@@ -744,16 +749,16 @@
         <v>1</v>
       </c>
       <c r="C11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11">
         <v>0.05</v>
-      </c>
-      <c r="D11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>0.2</v>
       </c>
       <c r="H11" t="s">
         <v>4</v>
@@ -776,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="C12">
-        <v>1.1000000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -785,7 +790,7 @@
         <v>2</v>
       </c>
       <c r="G12">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="H12" t="s">
         <v>4</v>
@@ -807,7 +812,7 @@
       <c r="B13" s="10"/>
       <c r="C13" s="10">
         <f>C12*C7+C11*C9</f>
-        <v>20.950000000000003</v>
+        <v>1.3200000000000003</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>12</v>
@@ -816,7 +821,7 @@
       <c r="F13" s="10"/>
       <c r="G13" s="10">
         <f>G11*G9+G12*G7</f>
-        <v>12.100000000000001</v>
+        <v>0.9</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>12</v>
@@ -839,7 +844,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2">
         <f>C11*(1-$C$7/$C$6)+(C12-$C$8)*$C$7/$C$6</f>
-        <v>9.7500000000000087E-2</v>
+        <v>-0.23400000000000004</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>4</v>
@@ -848,7 +853,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2">
         <f>G11*(1-G7/G6)+(G12-G8)*G7/G6</f>
-        <v>0.15500000000000005</v>
+        <v>-3.4999999999999996E-2</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>4</v>
@@ -857,7 +862,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2">
         <f>K11*(1-K7/K6)+(K12-K8)*K7/K6</f>
-        <v>-0.7433333333333334</v>
+        <v>-0.55666666666666687</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>4</v>
@@ -870,18 +875,18 @@
       </c>
       <c r="C16">
         <f>C15</f>
-        <v>9.7500000000000087E-2</v>
+        <v>-0.23400000000000004</v>
       </c>
       <c r="D16">
         <f>C11+$A$12*(C12-C8)*C7/C9</f>
-        <v>0.05</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F16" t="s">
         <v>1</v>
       </c>
       <c r="G16">
-        <f>G15</f>
-        <v>0.15500000000000005</v>
+        <f>MAX(G15,0)</f>
+        <v>0</v>
       </c>
       <c r="J16" t="s">
         <v>1</v>
@@ -897,18 +902,18 @@
       </c>
       <c r="C17">
         <f>C8+C15</f>
-        <v>1.0975000000000001</v>
+        <v>2.766</v>
       </c>
       <c r="D17">
         <f>C12-$A$12*(C12-C8)</f>
-        <v>1.1000000000000001</v>
+        <v>0.03</v>
       </c>
       <c r="F17" t="s">
         <v>2</v>
       </c>
       <c r="G17">
         <f>G8+G15</f>
-        <v>1.155</v>
+        <v>0.76500000000000001</v>
       </c>
       <c r="J17" t="s">
         <v>2</v>
@@ -925,7 +930,7 @@
       <c r="B18" s="12"/>
       <c r="C18" s="10">
         <f>C16*C9+C17*C7</f>
-        <v>20.950000000000003</v>
+        <v>1.3199999999999994</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>12</v>
@@ -934,7 +939,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="10">
         <f>G16*G9+G17*G7</f>
-        <v>12.1</v>
+        <v>1.53</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>12</v>
@@ -973,12 +978,11 @@
       <c r="B20" s="12"/>
       <c r="C20" s="2">
         <f>C16*(1-$C$7/$C$6)+(C17-$C$8)*$C$7/$C$6</f>
-        <v>9.7500000000000142E-2</v>
+        <v>-0.23400000000000004</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
-      <c r="G20" s="10"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -995,9 +999,16 @@
       <c r="C21" s="10"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="12"/>
+      <c r="F21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="10">
+        <f>G11*G9/G7</f>
+        <v>0.45</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>17</v>
+      </c>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="15">
@@ -1010,11 +1021,17 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="10"/>
+      <c r="C22" s="10">
+        <f>C12+C11/(C7/C9)</f>
+        <v>0.66000000000000014</v>
+      </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
-      <c r="G22" s="10"/>
+      <c r="G22" s="10">
+        <f>G21*2</f>
+        <v>0.9</v>
+      </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
@@ -1027,10 +1044,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="10">
-        <f>SQRT(9.8*0.05)</f>
-        <v>0.70000000000000007</v>
+      <c r="B23" s="14"/>
+      <c r="C23" s="15">
+        <f>C22*2</f>
+        <v>1.3200000000000003</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -1045,12 +1062,15 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="10"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="10"/>
+      <c r="G24" s="10">
+        <f>G12+G11*(G9/G7)</f>
+        <v>0.45</v>
+      </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -1060,8 +1080,8 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="10"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -1075,8 +1095,8 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="10"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
@@ -1119,10 +1139,7 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="D29">
-        <f>D16*C9+D17*C7</f>
-        <v>20.950000000000003</v>
-      </c>
+      <c r="D29" s="12"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B31" t="s">

</xml_diff>

<commit_message>
//VJ 170210 FIX BUG: - stemflow causes MB error and drowned interception also. - channel overlfow whlevel < 0, no movement - channelDX = DX - Clean up some code
</commit_message>
<xml_diff>
--- a/docs/floodchannel.xlsx
+++ b/docs/floodchannel.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prgc\lisem\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="96" windowWidth="8592" windowHeight="8256" tabRatio="541"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="8595" windowHeight="8250" tabRatio="541"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -246,6 +251,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -293,7 +301,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -328,7 +336,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,16 +547,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -556,7 +564,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -564,7 +572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="4" t="s">
         <v>0</v>
@@ -588,7 +596,7 @@
       </c>
       <c r="J6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
         <v>5</v>
@@ -612,7 +620,7 @@
       </c>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="6" t="s">
         <v>3</v>
@@ -636,7 +644,7 @@
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="8" t="s">
         <v>6</v>
@@ -662,7 +670,7 @@
       </c>
       <c r="J9" s="8"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>13</v>
@@ -686,7 +694,7 @@
       </c>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6" t="s">
         <v>16</v>
@@ -703,7 +711,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6" t="s">
         <v>17</v>
@@ -720,7 +728,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>1</v>
       </c>
@@ -740,7 +748,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>2</v>
       </c>
@@ -760,7 +768,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
@@ -786,7 +794,7 @@
       </c>
       <c r="J15" s="9"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -812,7 +820,7 @@
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -842,7 +850,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -866,7 +874,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>12</v>
       </c>
@@ -892,7 +900,7 @@
       </c>
       <c r="J20" s="11"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>15</v>
       </c>
@@ -918,7 +926,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="11"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>2</v>
@@ -940,7 +948,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="11"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9">
@@ -962,7 +970,7 @@
       </c>
       <c r="J23" s="11"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>21</v>
@@ -974,7 +982,7 @@
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="12" t="s">
         <v>18</v>
@@ -986,7 +994,7 @@
       <c r="D25" s="11"/>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12" t="s">
         <v>19</v>
@@ -998,7 +1006,7 @@
       <c r="D26" s="11"/>
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
         <v>20</v>
@@ -1010,41 +1018,41 @@
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="13"/>
       <c r="D28" s="11"/>
       <c r="E28" s="11"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="9"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="9"/>
       <c r="D30" s="11"/>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D31" s="11"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="4" t="s">
         <v>0</v>
@@ -1057,20 +1065,20 @@
       </c>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C36" s="6">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E36" s="6"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="6" t="s">
         <v>3</v>
@@ -1083,107 +1091,107 @@
       </c>
       <c r="E37" s="6"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="8">
         <f>C35-C36</f>
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D38" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>1</v>
       </c>
       <c r="C39">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="D39" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>2</v>
       </c>
       <c r="C40">
-        <v>1.8</v>
+        <v>0.1</v>
       </c>
       <c r="D40" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="9">
         <f>C40*C36+C39*C38</f>
-        <v>34.900000000000006</v>
+        <v>3.5</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E41" s="9"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2">
         <f>C39*(1-C36/C35)+(C40-C37)*C36/C35</f>
-        <v>0.79500000000000004</v>
+        <v>-7.4999999999999983E-2</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>1</v>
       </c>
       <c r="C44">
         <f>C43</f>
-        <v>0.79500000000000004</v>
+        <v>-7.4999999999999983E-2</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>2</v>
       </c>
       <c r="C45">
         <f>C37+C43</f>
-        <v>1.7949999999999999</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="D45">
         <f>C40+C39*C38/C36</f>
-        <v>1.8368421052631578</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>12</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="9">
         <f>C44*C38+C45*C36</f>
-        <v>34.9</v>
+        <v>3.5</v>
       </c>
       <c r="D46" s="9">
         <f>D45*C36+D44*C38</f>
-        <v>34.9</v>
+        <v>3.5</v>
       </c>
       <c r="E46" s="11"/>
     </row>
@@ -1199,7 +1207,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1211,7 +1219,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>